<commit_message>
[GEN MCU] PWM Review data update
</commit_message>
<xml_diff>
--- a/Plasma LF Design Review Data.xlsx
+++ b/Plasma LF Design Review Data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Origin Gen" sheetId="1" r:id="rId1"/>
     <sheet name="GEN_MAIN" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Set-up" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
   <si>
     <t>Power[W]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,23 +110,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. 220VAC to 220VDC regulator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vout = 300VDC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vin = 220VAC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. Current transducer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0A에서 Vout=2.5V</t>
+    <t>VDC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>transformer turn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -134,31 +126,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1. 220VAC regulation된 출력이 300VDC이며, transformer 1:5 turn을 거쳐 1500VDC가 출력됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Current transduce가 전류 0A에서 Vout=2.5V이며,  Vout이 2.75V 이므로 소모 전류는 2.5A 이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vout_current trans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VDC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Iout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VDC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turn 1:5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Full P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Setup P</t>
+    <t>3. 5msec 기준으로 전체 Power는 1500VDC x 2.5A = 3750W 이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -166,7 +166,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>On-time</t>
+    <t>W/5msec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W/msec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W/usec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>On time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. PWM의 duty가 10%이므로 1usec당 10%만 On 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 위의 수식은 1개 Channel에 대한 Power이므로 PWM Pulse가 2개 channel이므로 실제 Power 계산시에는 두배를 해주어야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   PWM의 frequency가 변하더라도 duty는 10%를 유지하므로, Power는 Frequency와 무관하다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -174,19 +198,91 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>usec/1W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Full Time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Power control이 되는 한 주기의 time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 power</t>
+    <t>usec/W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power per usec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>On time per Power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>On time에 따른 Power 계산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power에 따른 On time 계산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>measure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frequency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Typ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Power 계산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_in</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -237,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -464,11 +560,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -476,15 +587,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -542,9 +644,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -846,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P45"/>
+  <dimension ref="B1:U58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -859,31 +990,37 @@
     <col min="4" max="4" width="16.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.875" customWidth="1"/>
     <col min="10" max="10" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="17.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="14"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C4" s="7" t="s">
+      <c r="C3" s="11"/>
+      <c r="K3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="15">
         <v>10</v>
       </c>
       <c r="F4" s="1">
@@ -895,13 +1032,22 @@
       <c r="H4" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="8"/>
-      <c r="D5" s="23" t="s">
+      <c r="M4" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="41"/>
+      <c r="D5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="16">
         <v>50</v>
       </c>
       <c r="F5" s="3">
@@ -913,15 +1059,27 @@
       <c r="H5" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C6" s="7" t="s">
+      <c r="L5" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="1">
+        <v>300</v>
+      </c>
+      <c r="N5" s="1">
+        <v>220</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="15">
         <v>50</v>
       </c>
       <c r="F6" s="1">
@@ -933,13 +1091,25 @@
       <c r="H6" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C7" s="9"/>
-      <c r="D7" s="24" t="s">
+      <c r="L6" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="5">
+        <v>5</v>
+      </c>
+      <c r="N6" s="5">
+        <v>5</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="42"/>
+      <c r="D7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="17">
         <v>2</v>
       </c>
       <c r="F7" s="5">
@@ -951,13 +1121,27 @@
       <c r="H7" s="6">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C8" s="9"/>
-      <c r="D8" s="24" t="s">
+      <c r="L7" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="3">
+        <f>M5*M6</f>
+        <v>1500</v>
+      </c>
+      <c r="N7" s="3">
+        <f>N5*N6</f>
+        <v>1100</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C8" s="42"/>
+      <c r="D8" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="17">
         <v>5</v>
       </c>
       <c r="F8" s="5">
@@ -970,56 +1154,104 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C9" s="9"/>
-      <c r="D9" s="24" t="s">
+    <row r="9" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="42"/>
+      <c r="D9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="18">
         <v>82</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>182</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>900</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="9">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="8"/>
-      <c r="D10" s="23" t="s">
+      <c r="K9" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="41"/>
+      <c r="D10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="23">
         <v>10</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="27">
+      <c r="G10" s="23"/>
+      <c r="H10" s="24">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
+      <c r="L10" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="3">
+        <f>(M10-2.5)*10</f>
+        <v>2.5</v>
+      </c>
+      <c r="N11" s="3">
+        <f>(N10-2.5)*10</f>
+        <v>2.5</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K13" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="34" t="s">
+      <c r="D14" s="10"/>
+      <c r="L14" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="1">
+        <f>M7*M11</f>
+        <v>3750</v>
+      </c>
+      <c r="N14" s="1">
+        <f>N7*N11</f>
+        <v>2750</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="32" t="s">
         <v>3</v>
       </c>
       <c r="E15">
@@ -1028,35 +1260,30 @@
       <c r="F15">
         <v>3000</v>
       </c>
-      <c r="J15" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="N15" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="O15" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="P15" s="35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C16" s="15">
+      <c r="L15" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" s="5">
+        <f>M14/5</f>
+        <v>750</v>
+      </c>
+      <c r="N15" s="5">
+        <f>N14/5</f>
+        <v>550</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="12">
         <v>1</v>
       </c>
       <c r="D16" s="2">
         <f>C16*9</f>
         <v>9</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="25">
         <f>D16/$E$15</f>
         <v>1.8E-3</v>
       </c>
@@ -1064,37 +1291,30 @@
         <f>E16*$F$15</f>
         <v>5.3999999999999995</v>
       </c>
-      <c r="J16" s="15">
-        <v>10</v>
-      </c>
-      <c r="K16" s="2">
-        <v>90</v>
-      </c>
-      <c r="M16" s="15">
-        <v>10</v>
-      </c>
-      <c r="N16" s="40">
-        <f>1/M16*1000</f>
-        <v>100</v>
-      </c>
-      <c r="O16" s="40">
-        <f>N16*0.5</f>
-        <v>50</v>
-      </c>
-      <c r="P16" s="41">
-        <f t="shared" ref="P16:P19" si="0">N16*0.1</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C17" s="16">
+      <c r="L16" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="3">
+        <f>M15/1000</f>
+        <v>0.75</v>
+      </c>
+      <c r="N16" s="3">
+        <f>N15/1000</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C17" s="13">
         <v>100</v>
       </c>
       <c r="D17" s="6">
         <f>C17*9</f>
         <v>900</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="25">
         <f>D17/$E$15</f>
         <v>0.18</v>
       </c>
@@ -1102,37 +1322,16 @@
         <f>E17*$F$15</f>
         <v>540</v>
       </c>
-      <c r="J17" s="16">
-        <v>20</v>
-      </c>
-      <c r="K17" s="6">
-        <v>180</v>
-      </c>
-      <c r="M17" s="16">
-        <v>20</v>
-      </c>
-      <c r="N17" s="29">
-        <f t="shared" ref="N17:N25" si="1">1/M17*1000</f>
-        <v>50</v>
-      </c>
-      <c r="O17" s="29">
-        <f t="shared" ref="O17:O25" si="2">N17*0.5</f>
-        <v>25</v>
-      </c>
-      <c r="P17" s="42">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="17">
+    </row>
+    <row r="18" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="14">
         <v>550</v>
       </c>
       <c r="D18" s="4">
         <f>C18*9</f>
         <v>4950</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="25">
         <f>D18/$E$15</f>
         <v>0.99</v>
       </c>
@@ -1140,105 +1339,42 @@
         <f>E18*$F$15</f>
         <v>2970</v>
       </c>
-      <c r="J18" s="16">
-        <v>30</v>
-      </c>
-      <c r="K18" s="6">
-        <v>270</v>
-      </c>
-      <c r="M18" s="16">
-        <v>30</v>
-      </c>
-      <c r="N18" s="29">
-        <f t="shared" si="1"/>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="O18" s="29">
-        <f t="shared" si="2"/>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="P18" s="42">
-        <f t="shared" si="0"/>
-        <v>3.3333333333333339</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J19" s="16">
-        <v>40</v>
-      </c>
-      <c r="K19" s="6">
-        <v>360</v>
-      </c>
-      <c r="M19" s="16">
-        <v>40</v>
-      </c>
-      <c r="N19" s="29">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="O19" s="29">
-        <f t="shared" si="2"/>
-        <v>12.5</v>
-      </c>
-      <c r="P19" s="42">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+      <c r="K18" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K19" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="16">
-        <v>50</v>
-      </c>
-      <c r="K20" s="6">
-        <v>450</v>
-      </c>
-      <c r="M20" s="16">
-        <v>50</v>
-      </c>
-      <c r="N20" s="29">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="O20" s="29">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="P20" s="42">
-        <f>N20*0.1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L20" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="45">
+        <f>M16*0.1</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="N20" s="45">
+        <f>N16*0.1</f>
+        <v>5.5000000000000007E-2</v>
+      </c>
+      <c r="O20" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="U20" s="7"/>
+    </row>
+    <row r="21" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="16">
-        <v>60</v>
-      </c>
-      <c r="K21" s="6">
-        <v>540</v>
-      </c>
-      <c r="M21" s="16">
-        <v>60</v>
-      </c>
-      <c r="N21" s="29">
-        <f t="shared" si="1"/>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="O21" s="29">
-        <f t="shared" si="2"/>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="P21" s="42">
-        <f t="shared" ref="P21:P25" si="3">N21*0.1</f>
-        <v>1.666666666666667</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C22" s="31" t="s">
+    </row>
+    <row r="22" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="28" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="1">
@@ -1247,299 +1383,573 @@
       <c r="E22" s="1">
         <v>30</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="16">
-        <v>70</v>
-      </c>
-      <c r="K22" s="6">
-        <v>630</v>
-      </c>
-      <c r="M22" s="16">
-        <v>70</v>
-      </c>
-      <c r="N22" s="29">
-        <f t="shared" si="1"/>
-        <v>14.285714285714285</v>
-      </c>
-      <c r="O22" s="29">
-        <f t="shared" si="2"/>
-        <v>7.1428571428571423</v>
-      </c>
-      <c r="P22" s="42">
-        <f t="shared" si="3"/>
-        <v>1.4285714285714286</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C23" s="32" t="s">
+      <c r="K22" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C23" s="29" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="5">
         <f>1/(D22*1000)*1000000</f>
         <v>20</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="26">
         <f>1/(E22*1000)*1000000</f>
         <v>33.333333333333336</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="16">
-        <v>80</v>
-      </c>
-      <c r="K23" s="6">
-        <v>720</v>
-      </c>
-      <c r="M23" s="16">
-        <v>80</v>
-      </c>
-      <c r="N23" s="29">
-        <f>1/M23*1000</f>
-        <v>12.5</v>
-      </c>
-      <c r="O23" s="29">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="P23" s="42">
-        <f t="shared" si="3"/>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C24" s="32" t="s">
+      <c r="L23" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="M23" s="1">
+        <f>M20*2</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N23" s="1">
+        <f>N20*2</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="29" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="5">
         <f>D23*0.5</f>
         <v>10</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="26">
         <f>E23*0.5</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="F24" s="37" t="s">
+      <c r="F24" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="16">
-        <v>90</v>
-      </c>
-      <c r="K24" s="6">
-        <v>810</v>
-      </c>
-      <c r="M24" s="16">
-        <v>90</v>
-      </c>
-      <c r="N24" s="29">
-        <f t="shared" si="1"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="O24" s="29">
-        <f t="shared" si="2"/>
-        <v>5.5555555555555554</v>
-      </c>
-      <c r="P24" s="42">
-        <f t="shared" si="3"/>
-        <v>1.1111111111111112</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="33" t="s">
+      <c r="L24" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="M24" s="44">
+        <f>1/M23</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="N24" s="44">
+        <f>1/N23</f>
+        <v>9.0909090909090899</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="3">
         <f>D23*0.1</f>
         <v>2</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="27">
         <f>E23*0.1</f>
         <v>3.3333333333333339</v>
       </c>
-      <c r="F25" s="38" t="s">
+      <c r="F25" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="16">
+    </row>
+    <row r="26" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K26" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L27" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="M27" s="1">
+        <v>10</v>
+      </c>
+      <c r="N27" s="1">
         <v>100</v>
       </c>
-      <c r="K25" s="6">
+      <c r="O27" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="27">
+        <f>M$24*M27</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="N28" s="27">
+        <f>N$24*N27</f>
+        <v>909.09090909090901</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="12">
+        <v>10</v>
+      </c>
+      <c r="D29" s="2">
+        <v>90</v>
+      </c>
+      <c r="F29" s="13">
+        <v>20</v>
+      </c>
+      <c r="G29" s="26">
+        <f t="shared" ref="G29:G37" si="0">1/F29*1000</f>
+        <v>50</v>
+      </c>
+      <c r="H29" s="26">
+        <f t="shared" ref="H29:H37" si="1">G29*0.5</f>
+        <v>25</v>
+      </c>
+      <c r="I29" s="38">
+        <f t="shared" ref="I29:I31" si="2">G29*0.1</f>
+        <v>5</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="N29" s="43"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C30" s="13">
+        <v>20</v>
+      </c>
+      <c r="D30" s="6">
+        <v>180</v>
+      </c>
+      <c r="F30" s="13">
+        <v>30</v>
+      </c>
+      <c r="G30" s="26">
+        <f t="shared" si="0"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="H30" s="26">
+        <f t="shared" si="1"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="I30" s="38">
+        <f t="shared" si="2"/>
+        <v>3.3333333333333339</v>
+      </c>
+      <c r="L30" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="M30" s="37">
+        <v>90</v>
+      </c>
+      <c r="N30" s="37">
         <v>900</v>
       </c>
-      <c r="M25" s="17">
-        <v>100</v>
-      </c>
-      <c r="N25" s="30">
+      <c r="O30" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="13">
+        <v>30</v>
+      </c>
+      <c r="D31" s="6">
+        <v>270</v>
+      </c>
+      <c r="F31" s="13">
+        <v>40</v>
+      </c>
+      <c r="G31" s="26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H31" s="26">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="I31" s="38">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="L31" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="M31" s="3">
+        <f>M$23*M30</f>
+        <v>13.500000000000002</v>
+      </c>
+      <c r="N31" s="3">
+        <f>N$23*N30</f>
+        <v>99.000000000000014</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="13">
+        <v>40</v>
+      </c>
+      <c r="D32" s="6">
+        <v>360</v>
+      </c>
+      <c r="F32" s="13">
+        <v>50</v>
+      </c>
+      <c r="G32" s="26">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H32" s="26">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="O25" s="30">
-        <f t="shared" si="2"/>
+      <c r="I32" s="38">
+        <f>G32*0.1</f>
+        <v>2</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C33" s="13">
+        <v>50</v>
+      </c>
+      <c r="D33" s="6">
+        <v>450</v>
+      </c>
+      <c r="F33" s="13">
+        <v>60</v>
+      </c>
+      <c r="G33" s="26">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H33" s="26">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="I33" s="38">
+        <f t="shared" ref="I33:I37" si="3">G33*0.1</f>
+        <v>1.666666666666667</v>
+      </c>
+      <c r="L33" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" s="1">
+        <v>300</v>
+      </c>
+      <c r="N33" s="1">
+        <v>220</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="13">
+        <v>60</v>
+      </c>
+      <c r="D34" s="6">
+        <v>540</v>
+      </c>
+      <c r="F34" s="13">
+        <v>70</v>
+      </c>
+      <c r="G34" s="26">
+        <f t="shared" si="0"/>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="H34" s="26">
+        <f t="shared" si="1"/>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="I34" s="38">
+        <f t="shared" si="3"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="L34" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="M34" s="3">
+        <f>M14/M33</f>
+        <v>12.5</v>
+      </c>
+      <c r="N34" s="3">
+        <f>N14/N33</f>
+        <v>12.5</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C35" s="13">
+        <v>70</v>
+      </c>
+      <c r="D35" s="6">
+        <v>630</v>
+      </c>
+      <c r="F35" s="13">
+        <v>80</v>
+      </c>
+      <c r="G35" s="26">
+        <f>1/F35*1000</f>
+        <v>12.5</v>
+      </c>
+      <c r="H35" s="26">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+      <c r="I35" s="38">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C36" s="13">
+        <v>80</v>
+      </c>
+      <c r="D36" s="6">
+        <v>720</v>
+      </c>
+      <c r="F36" s="13">
+        <v>90</v>
+      </c>
+      <c r="G36" s="26">
+        <f t="shared" si="0"/>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="H36" s="26">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="I36" s="38">
+        <f t="shared" si="3"/>
+        <v>1.1111111111111112</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="13">
+        <v>90</v>
+      </c>
+      <c r="D37" s="6">
+        <v>810</v>
+      </c>
+      <c r="F37" s="14">
+        <v>100</v>
+      </c>
+      <c r="G37" s="27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H37" s="27">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="P25" s="43">
+      <c r="I37" s="39">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J26" s="16">
+    <row r="38" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C38" s="13">
+        <v>100</v>
+      </c>
+      <c r="D38" s="6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C39" s="13">
         <v>110</v>
       </c>
-      <c r="K26" s="6">
+      <c r="D39" s="6">
         <v>990</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J27" s="16">
+    <row r="40" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C40" s="13">
         <v>120</v>
       </c>
-      <c r="K27" s="6">
+      <c r="D40" s="6">
         <v>1080</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J28" s="16">
+    <row r="41" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C41" s="13">
         <v>130</v>
       </c>
-      <c r="K28" s="6">
+      <c r="D41" s="6">
         <v>1170</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J29" s="16">
+    <row r="42" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C42" s="13">
         <v>140</v>
       </c>
-      <c r="K29" s="6">
+      <c r="D42" s="6">
         <v>1260</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J30" s="16">
+    <row r="43" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C43" s="13">
         <v>150</v>
       </c>
-      <c r="K30" s="6">
+      <c r="D43" s="6">
         <v>1350</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J31" s="16">
+    <row r="44" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C44" s="13">
         <v>160</v>
       </c>
-      <c r="K31" s="6">
+      <c r="D44" s="6">
         <v>1440</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J32" s="16">
+    <row r="45" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C45" s="13">
         <v>170</v>
       </c>
-      <c r="K32" s="6">
+      <c r="D45" s="6">
         <v>1530</v>
       </c>
     </row>
-    <row r="33" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J33" s="16">
+    <row r="46" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C46" s="13">
         <v>180</v>
       </c>
-      <c r="K33" s="6">
+      <c r="D46" s="6">
         <v>1620</v>
       </c>
     </row>
-    <row r="34" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J34" s="16">
+    <row r="47" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C47" s="13">
         <v>190</v>
       </c>
-      <c r="K34" s="6">
+      <c r="D47" s="6">
         <v>1710</v>
       </c>
     </row>
-    <row r="35" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J35" s="16">
+    <row r="48" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C48" s="13">
         <v>200</v>
       </c>
-      <c r="K35" s="6">
+      <c r="D48" s="6">
         <v>1800</v>
       </c>
     </row>
-    <row r="36" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J36" s="16">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C49" s="13">
         <v>210</v>
       </c>
-      <c r="K36" s="6">
+      <c r="D49" s="6">
         <v>1890</v>
       </c>
     </row>
-    <row r="37" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J37" s="16">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C50" s="13">
         <v>220</v>
       </c>
-      <c r="K37" s="6">
+      <c r="D50" s="6">
         <v>1980</v>
       </c>
     </row>
-    <row r="38" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J38" s="16">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C51" s="13">
         <v>230</v>
       </c>
-      <c r="K38" s="6">
+      <c r="D51" s="6">
         <v>2070</v>
       </c>
     </row>
-    <row r="39" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J39" s="16">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="13">
         <v>240</v>
       </c>
-      <c r="K39" s="6">
+      <c r="D52" s="6">
         <v>2160</v>
       </c>
     </row>
-    <row r="40" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J40" s="16">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C53" s="13">
         <v>250</v>
       </c>
-      <c r="K40" s="6">
+      <c r="D53" s="6">
         <v>2250</v>
       </c>
     </row>
-    <row r="41" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J41" s="16">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="13">
         <v>260</v>
       </c>
-      <c r="K41" s="6">
+      <c r="D54" s="6">
         <v>2340</v>
       </c>
     </row>
-    <row r="42" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J42" s="16">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C55" s="13">
         <v>270</v>
       </c>
-      <c r="K42" s="6">
+      <c r="D55" s="6">
         <v>2430</v>
       </c>
     </row>
-    <row r="43" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J43" s="16">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C56" s="13">
         <v>280</v>
       </c>
-      <c r="K43" s="6">
+      <c r="D56" s="6">
         <v>2520</v>
       </c>
     </row>
-    <row r="44" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J44" s="16">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C57" s="13">
         <v>290</v>
       </c>
-      <c r="K44" s="6">
+      <c r="D57" s="6">
         <v>2610</v>
       </c>
     </row>
-    <row r="45" spans="10:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J45" s="17">
+    <row r="58" spans="3:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C58" s="14">
         <v>300</v>
       </c>
-      <c r="K45" s="4">
+      <c r="D58" s="4">
         <v>2700</v>
       </c>
     </row>
@@ -1556,204 +1966,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L22"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="5.125" style="14" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3">
-        <v>220</v>
-      </c>
-      <c r="G3">
-        <f>F3*5</f>
-        <v>1100</v>
-      </c>
-      <c r="H3">
-        <f>-G3</f>
-        <v>-1100</v>
-      </c>
-      <c r="I3">
-        <v>0.25</v>
-      </c>
-      <c r="J3">
-        <f>I3*10</f>
-        <v>2.5</v>
-      </c>
-      <c r="K3">
-        <f>G3*J3</f>
-        <v>2750</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4">
-        <v>300</v>
-      </c>
-      <c r="G4">
-        <f>F4*5</f>
-        <v>1500</v>
-      </c>
-      <c r="H4">
-        <f>-G4</f>
-        <v>-1500</v>
-      </c>
-      <c r="I4">
-        <v>0.25</v>
-      </c>
-      <c r="J4">
-        <f>I4*10</f>
-        <v>2.5</v>
-      </c>
-      <c r="K4">
-        <f>G4*J4</f>
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10">
-        <v>300</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I11" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11">
-        <f>J10*5</f>
-        <v>1500</v>
-      </c>
-      <c r="K11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12">
-        <v>2.5</v>
-      </c>
-      <c r="K12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13">
-        <f>J12*J11</f>
-        <v>3750</v>
-      </c>
-      <c r="K13" t="s">
-        <v>36</v>
-      </c>
-      <c r="L13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14">
-        <v>5000</v>
-      </c>
-      <c r="K14" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I15" t="s">
-        <v>37</v>
-      </c>
-      <c r="J15">
-        <f>9/J14</f>
-        <v>1.8E-3</v>
-      </c>
-      <c r="K15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J20">
-        <v>100</v>
-      </c>
-      <c r="K20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21">
-        <f>9/5000</f>
-        <v>1.8E-3</v>
-      </c>
-      <c r="K21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I22" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22">
-        <f>J20*J21</f>
-        <v>0.18</v>
-      </c>
-      <c r="K22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1761,12 +1984,90 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="8.125" style="55" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="55" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="54"/>
+      <c r="C5" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[GEN MCU] Pspice file 추가
</commit_message>
<xml_diff>
--- a/Plasma LF Design Review Data.xlsx
+++ b/Plasma LF Design Review Data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="GEN_MAIN" sheetId="2" r:id="rId2"/>
     <sheet name="Set-up" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -646,15 +646,6 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -673,6 +664,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -685,6 +685,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -733,7 +736,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -768,7 +771,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -979,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1014,7 +1017,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="52" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -1038,12 +1041,12 @@
       <c r="N4" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="52" t="s">
+      <c r="O4" s="49" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="41"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="20" t="s">
         <v>1</v>
       </c>
@@ -1059,7 +1062,7 @@
       <c r="H5" s="4">
         <v>30</v>
       </c>
-      <c r="L5" s="47" t="s">
+      <c r="L5" s="44" t="s">
         <v>24</v>
       </c>
       <c r="M5" s="1">
@@ -1073,7 +1076,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="52" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="19" t="s">
@@ -1091,7 +1094,7 @@
       <c r="H6" s="2">
         <v>30</v>
       </c>
-      <c r="L6" s="48" t="s">
+      <c r="L6" s="45" t="s">
         <v>25</v>
       </c>
       <c r="M6" s="5">
@@ -1105,7 +1108,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="42"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="21" t="s">
         <v>10</v>
       </c>
@@ -1121,7 +1124,7 @@
       <c r="H7" s="6">
         <v>3.2</v>
       </c>
-      <c r="L7" s="49" t="s">
+      <c r="L7" s="46" t="s">
         <v>26</v>
       </c>
       <c r="M7" s="3">
@@ -1137,7 +1140,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="42"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="21" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1158,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="42"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="21" t="s">
         <v>3</v>
       </c>
@@ -1176,7 +1179,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="41"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="20" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1193,7 @@
       <c r="H10" s="24">
         <v>6</v>
       </c>
-      <c r="L10" s="47" t="s">
+      <c r="L10" s="44" t="s">
         <v>30</v>
       </c>
       <c r="M10" s="1">
@@ -1204,7 +1207,7 @@
       </c>
     </row>
     <row r="11" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L11" s="49" t="s">
+      <c r="L11" s="46" t="s">
         <v>32</v>
       </c>
       <c r="M11" s="3">
@@ -1219,6 +1222,12 @@
         <v>33</v>
       </c>
     </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <f>1/E6</f>
+        <v>0.02</v>
+      </c>
+    </row>
     <row r="13" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="11" t="s">
         <v>14</v>
@@ -1232,7 +1241,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="L14" s="47" t="s">
+      <c r="L14" s="44" t="s">
         <v>35</v>
       </c>
       <c r="M14" s="1">
@@ -1260,7 +1269,7 @@
       <c r="F15">
         <v>3000</v>
       </c>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="45" t="s">
         <v>35</v>
       </c>
       <c r="M15" s="5">
@@ -1291,7 +1300,7 @@
         <f>E16*$F$15</f>
         <v>5.3999999999999995</v>
       </c>
-      <c r="L16" s="49" t="s">
+      <c r="L16" s="46" t="s">
         <v>35</v>
       </c>
       <c r="M16" s="3">
@@ -1352,18 +1361,18 @@
       <c r="B20" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L20" s="50" t="s">
+      <c r="L20" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="M20" s="45">
+      <c r="M20" s="42">
         <f>M16*0.1</f>
         <v>7.5000000000000011E-2</v>
       </c>
-      <c r="N20" s="45">
+      <c r="N20" s="42">
         <f>N16*0.1</f>
         <v>5.5000000000000007E-2</v>
       </c>
-      <c r="O20" s="46" t="s">
+      <c r="O20" s="43" t="s">
         <v>39</v>
       </c>
       <c r="U20" s="7"/>
@@ -1405,7 +1414,7 @@
       <c r="F23" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="47" t="s">
+      <c r="L23" s="44" t="s">
         <v>46</v>
       </c>
       <c r="M23" s="1">
@@ -1435,14 +1444,14 @@
       <c r="F24" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="49" t="s">
+      <c r="L24" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="M24" s="44">
+      <c r="M24" s="41">
         <f>1/M23</f>
         <v>6.6666666666666661</v>
       </c>
-      <c r="N24" s="44">
+      <c r="N24" s="41">
         <f>1/N23</f>
         <v>9.0909090909090899</v>
       </c>
@@ -1472,7 +1481,7 @@
       </c>
     </row>
     <row r="27" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L27" s="47" t="s">
+      <c r="L27" s="44" t="s">
         <v>35</v>
       </c>
       <c r="M27" s="1">
@@ -1504,7 +1513,7 @@
       <c r="I28" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="L28" s="49" t="s">
+      <c r="L28" s="46" t="s">
         <v>40</v>
       </c>
       <c r="M28" s="27">
@@ -1544,7 +1553,7 @@
       <c r="K29" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="N29" s="43"/>
+      <c r="N29" s="40"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C30" s="13">
@@ -1568,7 +1577,7 @@
         <f t="shared" si="2"/>
         <v>3.3333333333333339</v>
       </c>
-      <c r="L30" s="47" t="s">
+      <c r="L30" s="44" t="s">
         <v>40</v>
       </c>
       <c r="M30" s="37">
@@ -1603,7 +1612,7 @@
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="L31" s="49" t="s">
+      <c r="L31" s="46" t="s">
         <v>35</v>
       </c>
       <c r="M31" s="3">
@@ -1666,7 +1675,7 @@
         <f t="shared" ref="I33:I37" si="3">G33*0.1</f>
         <v>1.666666666666667</v>
       </c>
-      <c r="L33" s="47" t="s">
+      <c r="L33" s="44" t="s">
         <v>24</v>
       </c>
       <c r="M33" s="1">
@@ -1701,7 +1710,7 @@
         <f t="shared" si="3"/>
         <v>1.4285714285714286</v>
       </c>
-      <c r="L34" s="49" t="s">
+      <c r="L34" s="46" t="s">
         <v>66</v>
       </c>
       <c r="M34" s="3">
@@ -1992,32 +2001,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.125" style="55" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" style="51" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="51" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="51" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="51" t="s">
+    <row r="2" spans="2:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="48" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="54"/>
+      <c r="C3" s="55"/>
       <c r="D3">
         <v>0</v>
       </c>
@@ -2029,10 +2038,10 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="51" t="s">
         <v>58</v>
       </c>
       <c r="D4">
@@ -2046,17 +2055,17 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55" t="s">
+      <c r="B5" s="55"/>
+      <c r="C5" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="50" t="s">
         <v>64</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="50" t="s">
         <v>64</v>
       </c>
       <c r="G5" s="7" t="s">

</xml_diff>

<commit_message>
[GEN MAIN] Pspice update
</commit_message>
<xml_diff>
--- a/Plasma LF Design Review Data.xlsx
+++ b/Plasma LF Design Review Data.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Origin Gen" sheetId="1" r:id="rId1"/>
     <sheet name="GEN_MAIN" sheetId="2" r:id="rId2"/>
     <sheet name="Set-up" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>Power[W]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -283,6 +284,82 @@
   </si>
   <si>
     <t>I_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Touch PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMFILE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CWV2-070BR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7인치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLASH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>512M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vendor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>베젤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPCV5-070WR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>128GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -290,11 +367,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="177" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +394,13 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -576,10 +661,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -676,8 +764,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -982,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -1978,7 +2071,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1048576"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2080,4 +2173,112 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.25" customWidth="1"/>
+    <col min="8" max="8" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="57"/>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="56">
+        <v>363000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="56">
+        <v>583000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[GEN MCU] Issue update
</commit_message>
<xml_diff>
--- a/Plasma LF Design Review Data.xlsx
+++ b/Plasma LF Design Review Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Origin Gen" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="Set-up" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
     <sheet name="Snubber" sheetId="5" r:id="rId5"/>
+    <sheet name="MCU" sheetId="6" r:id="rId6"/>
+    <sheet name="Current" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
   <si>
     <t>Power[W]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -381,6 +383,66 @@
   </si>
   <si>
     <t>V2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO VCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Origin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Origin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snubber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Load</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -393,7 +455,7 @@
     <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="177" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +486,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -688,7 +757,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -774,6 +843,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -787,6 +862,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1007,7 +1086,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1042,7 +1121,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1253,7 +1332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -1288,7 +1367,7 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="55" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -1317,7 +1396,7 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="54"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="20" t="s">
         <v>1</v>
       </c>
@@ -1347,7 +1426,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="55" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="19" t="s">
@@ -1379,7 +1458,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="55"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="21" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +1490,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="55"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="21" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1508,7 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="55"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="21" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1529,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="54"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="20" t="s">
         <v>4</v>
       </c>
@@ -2248,8 +2327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2271,89 +2350,142 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G5"/>
+  <dimension ref="B2:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="8.125" style="51" customWidth="1"/>
     <col min="3" max="3" width="10.125" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="7"/>
+    <col min="10" max="10" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="48" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="48" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="J2" s="54"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E4" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F4" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="56" t="s">
+      <c r="G4" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="61"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3">
+      <c r="C5" s="58"/>
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F5">
         <v>300</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>300</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="56" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C6" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>20</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>100</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="56"/>
-      <c r="C5" s="51" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="58"/>
+      <c r="C7" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D7" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="E5">
+      <c r="E7">
         <v>10</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F7" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G7" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:B5"/>
+  <mergeCells count="5">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2393,10 +2525,10 @@
       <c r="F2" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="57"/>
+      <c r="H2" s="59"/>
       <c r="I2" t="s">
         <v>73</v>
       </c>
@@ -2472,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2531,4 +2663,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="3.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="5">
+        <v>4.7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="5">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="60">
+        <f>D5*D7/(D6+D7)</f>
+        <v>3.4013605442176873</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>150</v>
+      </c>
+      <c r="C5">
+        <v>17.8</v>
+      </c>
+      <c r="D5">
+        <v>17.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[GEN MAIN] review data update
</commit_message>
<xml_diff>
--- a/Plasma LF Design Review Data.xlsx
+++ b/Plasma LF Design Review Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Origin Gen" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="MCU" sheetId="6" r:id="rId6"/>
     <sheet name="Current" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
   <si>
     <t>Power[W]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,10 +71,6 @@
   </si>
   <si>
     <t>LF Generator Set-up Item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Measure</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -443,6 +439,18 @@
   </si>
   <si>
     <t>Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Measure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ω</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -854,7 +862,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -932,7 +940,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -953,18 +960,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -985,12 +980,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -998,6 +987,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,12 +1014,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
@@ -1231,7 +1251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1266,7 +1286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1477,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1497,22 +1517,22 @@
     <col min="24" max="25" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="C3" s="11"/>
       <c r="K3" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="69" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -1531,17 +1551,20 @@
         <v>20</v>
       </c>
       <c r="M4" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="32" t="s">
+      <c r="O4" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="59"/>
+      <c r="T4" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="70"/>
       <c r="D5" s="20" t="s">
         <v>1</v>
       </c>
@@ -1558,7 +1581,7 @@
         <v>30</v>
       </c>
       <c r="L5" s="44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M5" s="1">
         <v>300</v>
@@ -1566,12 +1589,15 @@
       <c r="N5" s="1">
         <v>220</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C6" s="58" t="s">
+      <c r="O5" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C6" s="69" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="19" t="s">
@@ -1590,7 +1616,7 @@
         <v>30</v>
       </c>
       <c r="L6" s="45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M6" s="5">
         <v>5</v>
@@ -1598,12 +1624,15 @@
       <c r="N6" s="5">
         <v>5</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="60"/>
+      <c r="O6" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="T6" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="71"/>
       <c r="D7" s="21" t="s">
         <v>10</v>
       </c>
@@ -1620,7 +1649,7 @@
         <v>3.2</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M7" s="3">
         <f>M5*M6</f>
@@ -1630,12 +1659,15 @@
         <f>N5*N6</f>
         <v>1100</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="60"/>
+      <c r="O7" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="3">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C8" s="71"/>
       <c r="D8" s="21" t="s">
         <v>2</v>
       </c>
@@ -1652,8 +1684,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="60"/>
+    <row r="9" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="71"/>
       <c r="D9" s="21" t="s">
         <v>3</v>
       </c>
@@ -1670,11 +1702,11 @@
         <v>70</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="59"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="70"/>
       <c r="D10" s="20" t="s">
         <v>4</v>
       </c>
@@ -1689,7 +1721,7 @@
         <v>6</v>
       </c>
       <c r="L10" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M10" s="1">
         <v>2.75</v>
@@ -1698,12 +1730,15 @@
         <v>2.75</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" s="1">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="46" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L11" s="46" t="s">
-        <v>32</v>
       </c>
       <c r="M11" s="3">
         <f>(M10-2.5)*10</f>
@@ -1714,72 +1749,80 @@
         <v>2.5</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="T11" s="3">
+        <f>(T10-2.5)*10</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E12">
         <f>1/E6</f>
         <v>0.02</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" s="3">
+        <f>M7/M11</f>
+        <v>600</v>
+      </c>
+      <c r="N12" s="3">
+        <f>N7/N11</f>
+        <v>440</v>
+      </c>
+      <c r="O12" s="83" t="s">
+        <v>104</v>
+      </c>
+      <c r="T12" s="3">
+        <f>T7/T11</f>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="D14" s="10"/>
+      <c r="K14" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>5000</v>
+      </c>
+      <c r="F15">
+        <v>3000</v>
+      </c>
+      <c r="L15" s="44" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="L14" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="1">
+      <c r="M15" s="1">
         <f>M7*M11</f>
         <v>3750</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N15" s="1">
         <f>N7*N11</f>
         <v>2750</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>5000</v>
-      </c>
-      <c r="F15">
-        <v>3000</v>
-      </c>
-      <c r="L15" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="M15" s="5">
-        <f>M14/5</f>
-        <v>750</v>
-      </c>
-      <c r="N15" s="5">
-        <f>N14/5</f>
-        <v>550</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C16" s="12">
         <v>1</v>
       </c>
@@ -1795,22 +1838,22 @@
         <f>E16*$F$15</f>
         <v>5.3999999999999995</v>
       </c>
-      <c r="L16" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="3">
-        <f>M15/1000</f>
-        <v>0.75</v>
-      </c>
-      <c r="N16" s="3">
-        <f>N15/1000</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="L16" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="5">
+        <f>M15/5</f>
+        <v>750</v>
+      </c>
+      <c r="N16" s="5">
+        <f>N15/5</f>
+        <v>550</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="13">
         <v>100</v>
       </c>
@@ -1826,6 +1869,20 @@
         <f>E17*$F$15</f>
         <v>540</v>
       </c>
+      <c r="L17" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="3">
+        <f>M16/1000</f>
+        <v>0.75</v>
+      </c>
+      <c r="N17" s="3">
+        <f>N16/1000</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="14">
@@ -1843,43 +1900,43 @@
         <f>E18*$F$15</f>
         <v>2970</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="K19" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="M20" s="42">
-        <f>M16*0.1</f>
-        <v>7.5000000000000011E-2</v>
-      </c>
-      <c r="N20" s="42">
-        <f>N16*0.1</f>
-        <v>5.5000000000000007E-2</v>
-      </c>
-      <c r="O20" s="43" t="s">
-        <v>39</v>
+        <v>15</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="U20" s="7"/>
     </row>
     <row r="21" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="L21" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" s="42">
+        <f>M17*0.1</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="N21" s="42">
+        <f>N17*0.1</f>
+        <v>5.5000000000000007E-2</v>
+      </c>
+      <c r="O21" s="43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C22" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1">
         <v>50</v>
@@ -1888,15 +1945,12 @@
         <v>30</v>
       </c>
       <c r="F22" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="29" t="s">
         <v>18</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C23" s="29" t="s">
-        <v>19</v>
       </c>
       <c r="D23" s="5">
         <f>1/(D22*1000)*1000000</f>
@@ -1907,24 +1961,13 @@
         <v>33.333333333333336</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="M23" s="1">
-        <f>M20*2</f>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="N23" s="1">
-        <f>N20*2</f>
-        <v>0.11000000000000001</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C24" s="29" t="s">
         <v>11</v>
       </c>
@@ -1937,26 +1980,26 @@
         <v>16.666666666666668</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="M24" s="41">
-        <f>1/M23</f>
-        <v>6.6666666666666661</v>
-      </c>
-      <c r="N24" s="41">
-        <f>1/N23</f>
-        <v>9.0909090909090899</v>
-      </c>
-      <c r="O24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="44" t="s">
         <v>45</v>
+      </c>
+      <c r="M24" s="1">
+        <f>M21*2</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N24" s="1">
+        <f>N21*2</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C25" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="3">
         <f>D23*0.1</f>
@@ -1967,26 +2010,26 @@
         <v>3.3333333333333339</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K26" s="11" t="s">
-        <v>49</v>
+        <v>19</v>
+      </c>
+      <c r="L25" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="M25" s="41">
+        <f>1/M24</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="N25" s="41">
+        <f>1/N24</f>
+        <v>9.0909090909090899</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L27" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="M27" s="1">
-        <v>10</v>
-      </c>
-      <c r="N27" s="1">
-        <v>100</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>36</v>
+      <c r="K27" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2006,21 +2049,19 @@
         <v>11</v>
       </c>
       <c r="I28" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="M28" s="27">
-        <f>M$24*M27</f>
-        <v>66.666666666666657</v>
-      </c>
-      <c r="N28" s="27">
-        <f>N$24*N27</f>
-        <v>909.09090909090901</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>44</v>
+        <v>20</v>
+      </c>
+      <c r="L28" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="1">
+        <v>10</v>
+      </c>
+      <c r="N28" s="1">
+        <v>100</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2045,12 +2086,22 @@
         <f t="shared" ref="I29:I37" si="2">G29*0.1</f>
         <v>5</v>
       </c>
-      <c r="K29" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N29" s="40"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="L29" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="27">
+        <f>M$25*M28</f>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="N29" s="27">
+        <f>N$25*N28</f>
+        <v>909.09090909090901</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="13">
         <v>20</v>
       </c>
@@ -2072,20 +2123,12 @@
         <f t="shared" si="2"/>
         <v>3.3333333333333339</v>
       </c>
-      <c r="L30" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M30" s="37">
-        <v>90</v>
-      </c>
-      <c r="N30" s="37">
-        <v>900</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K30" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N30" s="40"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C31" s="13">
         <v>30</v>
       </c>
@@ -2107,19 +2150,17 @@
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="L31" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="M31" s="3">
-        <f>M$23*M30</f>
-        <v>13.500000000000002</v>
-      </c>
-      <c r="N31" s="3">
-        <f>N$23*N30</f>
-        <v>99.000000000000014</v>
-      </c>
-      <c r="O31" s="4" t="s">
-        <v>36</v>
+      <c r="L31" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31" s="37">
+        <v>90</v>
+      </c>
+      <c r="N31" s="37">
+        <v>900</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2144,11 +2185,22 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="K32" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L32" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" s="3">
+        <f>M$24*M31</f>
+        <v>13.500000000000002</v>
+      </c>
+      <c r="N32" s="3">
+        <f>N$24*N31</f>
+        <v>99.000000000000014</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="13">
         <v>50</v>
       </c>
@@ -2170,20 +2222,11 @@
         <f t="shared" si="2"/>
         <v>1.666666666666667</v>
       </c>
-      <c r="L33" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="M33" s="1">
-        <v>300</v>
-      </c>
-      <c r="N33" s="1">
-        <v>220</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K33" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C34" s="13">
         <v>60</v>
       </c>
@@ -2205,22 +2248,20 @@
         <f t="shared" si="2"/>
         <v>1.4285714285714286</v>
       </c>
-      <c r="L34" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="M34" s="3">
-        <f>M14/M33</f>
-        <v>12.5</v>
-      </c>
-      <c r="N34" s="3">
-        <f>N14/N33</f>
-        <v>12.5</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L34" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" s="1">
+        <v>300</v>
+      </c>
+      <c r="N34" s="1">
+        <v>220</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="13">
         <v>70</v>
       </c>
@@ -2241,6 +2282,20 @@
       <c r="I35" s="38">
         <f t="shared" si="2"/>
         <v>1.25</v>
+      </c>
+      <c r="L35" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="M35" s="3">
+        <f>M15/M34</f>
+        <v>12.5</v>
+      </c>
+      <c r="N35" s="3">
+        <f>N15/N34</f>
+        <v>12.5</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.3">
@@ -2483,7 +2538,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2497,91 +2552,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.125" style="50" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="50" customWidth="1"/>
+    <col min="2" max="2" width="8.125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="49" customWidth="1"/>
     <col min="10" max="10" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="J2" s="52"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="54"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="58" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="74"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="77" t="s">
+      <c r="H3" s="74"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="76" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" s="48" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="54"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="77"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="73"/>
+      <c r="D5" s="64">
+        <v>0</v>
+      </c>
+      <c r="E5" s="65"/>
+      <c r="F5" s="66">
+        <v>300</v>
+      </c>
+      <c r="G5" s="64">
+        <v>0</v>
+      </c>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66">
+        <v>300</v>
+      </c>
+      <c r="J5" s="67" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="58" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" s="48" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="78" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="78" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="79"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71">
-        <v>0</v>
-      </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="73">
-        <v>300</v>
-      </c>
-      <c r="G5" s="71">
-        <v>0</v>
-      </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="73">
-        <v>300</v>
-      </c>
-      <c r="J5" s="74" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>58</v>
       </c>
       <c r="D6" s="13">
         <v>20</v>
@@ -2597,69 +2652,69 @@
       <c r="I6" s="6">
         <v>100</v>
       </c>
-      <c r="J6" s="67" t="s">
-        <v>59</v>
+      <c r="J6" s="62" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="60"/>
-      <c r="C7" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>64</v>
+      <c r="B7" s="71"/>
+      <c r="C7" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>63</v>
       </c>
       <c r="E7" s="5">
         <v>10</v>
       </c>
-      <c r="F7" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="65" t="s">
-        <v>64</v>
+      <c r="F7" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>63</v>
       </c>
       <c r="H7" s="5">
         <v>10</v>
       </c>
-      <c r="I7" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="67" t="s">
+      <c r="I7" s="61" t="s">
         <v>63</v>
       </c>
+      <c r="J7" s="62" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="56"/>
-      <c r="C8" s="63"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="13"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
       <c r="G8" s="13"/>
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="67"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="56"/>
-      <c r="C9" s="63"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="13"/>
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
       <c r="G9" s="13"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="67"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="2:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="55"/>
-      <c r="C10" s="64"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="14"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="14"/>
       <c r="H10" s="3"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="68"/>
+      <c r="J10" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2697,81 +2752,81 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="78"/>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" s="50">
+        <v>363000</v>
+      </c>
+      <c r="F3" t="s">
         <v>69</v>
       </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="51">
-        <v>363000</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>70</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>71</v>
       </c>
-      <c r="H3" t="s">
-        <v>72</v>
-      </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="50">
+        <v>583000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" t="s">
         <v>81</v>
       </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="51">
-        <v>583000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" t="s">
-        <v>82</v>
-      </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2795,10 +2850,10 @@
   <sheetData>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
         <v>87</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
@@ -2830,10 +2885,10 @@
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
         <v>89</v>
-      </c>
-      <c r="D12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.3">
@@ -2863,52 +2918,52 @@
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="5">
         <v>5</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="5">
         <v>4.7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="5">
         <v>10</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="57">
+        <v>94</v>
+      </c>
+      <c r="D8" s="56">
         <f>D5*D7/(D6+D7)</f>
         <v>3.4013605442176873</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2929,13 +2984,13 @@
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
         <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>